<commit_message>
Formula for spiral wavelet
</commit_message>
<xml_diff>
--- a/source/source.xlsx
+++ b/source/source.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="-640" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-140" yWindow="9920" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -86,8 +86,32 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -97,11 +121,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="29">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -478,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B17" si="0" xml:space="preserve"> 1.2</f>
+        <f t="shared" ref="B3:B63" si="0" xml:space="preserve"> 1.2</f>
         <v>1.2</v>
       </c>
       <c r="C3">
@@ -710,6 +758,630 @@
         <v>5.2</v>
       </c>
       <c r="D17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <f xml:space="preserve"> 1.2</f>
+        <v>1.2</v>
+      </c>
+      <c r="C18">
+        <f>$B18+LOG($A18,2)</f>
+        <v>5.2874628412503402</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:C63" si="2">$B19+LOG($A19,2)</f>
+        <v>5.3699250014423123</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="2"/>
+        <v>5.4479275134435854</v>
+      </c>
+      <c r="D20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="2"/>
+        <v>5.5219280948873628</v>
+      </c>
+      <c r="D21">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C22">
+        <f t="shared" si="2"/>
+        <v>5.5923174227787609</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C23">
+        <f t="shared" si="2"/>
+        <v>5.6594316186372975</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C24">
+        <f t="shared" si="2"/>
+        <v>5.7235619560570132</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C25">
+        <f t="shared" si="2"/>
+        <v>5.7849625007211571</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C26">
+        <f t="shared" si="2"/>
+        <v>5.8438561897747245</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C27">
+        <f t="shared" si="2"/>
+        <v>5.9004397181410928</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C28">
+        <f t="shared" si="2"/>
+        <v>5.9548875021634693</v>
+      </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C29">
+        <f t="shared" si="2"/>
+        <v>6.0073549220576039</v>
+      </c>
+      <c r="D29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C30">
+        <f t="shared" si="2"/>
+        <v>6.0579809951275729</v>
+      </c>
+      <c r="D30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C31">
+        <f t="shared" si="2"/>
+        <v>6.1068905956085189</v>
+      </c>
+      <c r="D31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C32">
+        <f t="shared" si="2"/>
+        <v>6.154196310386876</v>
+      </c>
+      <c r="D32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C33">
+        <f>$B33+LOG($A33,2)</f>
+        <v>6.2</v>
+      </c>
+      <c r="D33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C34">
+        <f t="shared" si="2"/>
+        <v>6.2443941193584536</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C35">
+        <f t="shared" si="2"/>
+        <v>6.2874628412503402</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C36">
+        <f t="shared" si="2"/>
+        <v>6.3292830169449665</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C37">
+        <f t="shared" si="2"/>
+        <v>6.3699250014423123</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C38">
+        <f t="shared" si="2"/>
+        <v>6.4094533656289503</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C39">
+        <f t="shared" si="2"/>
+        <v>6.4479275134435854</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C40">
+        <f t="shared" si="2"/>
+        <v>6.4854022188622489</v>
+      </c>
+      <c r="D40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C41">
+        <f t="shared" si="2"/>
+        <v>6.5219280948873628</v>
+      </c>
+      <c r="D41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C42">
+        <f t="shared" si="2"/>
+        <v>6.557552004618084</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C43">
+        <f t="shared" si="2"/>
+        <v>6.5923174227787609</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C44">
+        <f t="shared" si="2"/>
+        <v>6.6262647547020981</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C45">
+        <f t="shared" si="2"/>
+        <v>6.6594316186372975</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C46">
+        <f t="shared" si="2"/>
+        <v>6.691853096329675</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C47">
+        <f t="shared" si="2"/>
+        <v>6.7235619560570132</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C48">
+        <f t="shared" si="2"/>
+        <v>6.7545888516776378</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C49">
+        <f t="shared" si="2"/>
+        <v>6.7849625007211571</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C50">
+        <f t="shared" si="2"/>
+        <v>6.8147098441152085</v>
+      </c>
+      <c r="D50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C51">
+        <f t="shared" si="2"/>
+        <v>6.8438561897747245</v>
+      </c>
+      <c r="D51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C52">
+        <f t="shared" si="2"/>
+        <v>6.8724253419714962</v>
+      </c>
+      <c r="D52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C53">
+        <f t="shared" si="2"/>
+        <v>6.9004397181410928</v>
+      </c>
+      <c r="D53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C54">
+        <f t="shared" si="2"/>
+        <v>6.9279204545631998</v>
+      </c>
+      <c r="D54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C55">
+        <f t="shared" si="2"/>
+        <v>6.9548875021634693</v>
+      </c>
+      <c r="D55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <f t="shared" si="0"/>
+        <v>1.2</v>
+      </c>
+      <c r="C56">
+        <f t="shared" si="2"/>
+        <v>6.9813597135246601</v>
+      </c>
+      <c r="D56">
         <v>2</v>
       </c>
     </row>

</xml_diff>